<commit_message>
Melhorias no sistema de Mala Direta.
</commit_message>
<xml_diff>
--- a/mala.xlsx
+++ b/mala.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>email</t>
   </si>
@@ -28,6 +28,144 @@
   </si>
   <si>
     <t>riatoso2@gmail.com</t>
+  </si>
+  <si>
+    <t>adm@darho.com.br</t>
+  </si>
+  <si>
+    <t>rh@homedock.com.br</t>
+  </si>
+  <si>
+    <t>vagas@macorganizacional.com.br</t>
+  </si>
+  <si>
+    <t>oportunidadesrecrutarh@gmail.com</t>
+  </si>
+  <si>
+    <t>rh@serquimica.com.br</t>
+  </si>
+  <si>
+    <t>rh@jsgrupo.com</t>
+  </si>
+  <si>
+    <t>rh@grupodigitalsaude.com.br</t>
+  </si>
+  <si>
+    <t>rh.recrutamentoararaquara@gmail.com</t>
+  </si>
+  <si>
+    <t>selecao2@grupoprovac.com.br</t>
+  </si>
+  <si>
+    <t>vagas@alpack.com.br</t>
+  </si>
+  <si>
+    <t>rh@shx.com.br</t>
+  </si>
+  <si>
+    <t>rh@tita.com.br</t>
+  </si>
+  <si>
+    <t>vagas@jnmoura.com.br</t>
+  </si>
+  <si>
+    <t>vagas.hyundairotem@outlook.com</t>
+  </si>
+  <si>
+    <t>selecaovarejo@wcabrasil.com.br</t>
+  </si>
+  <si>
+    <t>recrutamento.rao@resolv.com.br</t>
+  </si>
+  <si>
+    <t>rh@furacaopet.com.br</t>
+  </si>
+  <si>
+    <t>rh@bigdutchman.com.br</t>
+  </si>
+  <si>
+    <t>ger.rh@ahhbb.org.br</t>
+  </si>
+  <si>
+    <t>noeni.sandrini@grupobandeirantes.com.br</t>
+  </si>
+  <si>
+    <t>dp@eyetec.com.br</t>
+  </si>
+  <si>
+    <t>recrutamento@cambuhy.com.br</t>
+  </si>
+  <si>
+    <t>rh@polimetal.com.br</t>
+  </si>
+  <si>
+    <t>tgm-curiculo@weg.net</t>
+  </si>
+  <si>
+    <t>recutamento@essencialnutricao.com.br</t>
+  </si>
+  <si>
+    <t>recrutamento@jobterceirizacao.com.br</t>
+  </si>
+  <si>
+    <t>vagades@rissicontabilidade.com.br</t>
+  </si>
+  <si>
+    <t>carol.ventura@visualsystems.com.br</t>
+  </si>
+  <si>
+    <t>rh2021contrata@gmail.com</t>
+  </si>
+  <si>
+    <t>recrutamento@gsinima.com.br</t>
+  </si>
+  <si>
+    <t>recrutamento@colomboagroindustria.com.br</t>
+  </si>
+  <si>
+    <t>luciana@eventosrh.com.br</t>
+  </si>
+  <si>
+    <t>pessoas@stepwise.com.br</t>
+  </si>
+  <si>
+    <t>rhsimber@gmail.com</t>
+  </si>
+  <si>
+    <t>vagas.rc.sc@adoro.com.br</t>
+  </si>
+  <si>
+    <t>rh@route66.com.br</t>
+  </si>
+  <si>
+    <t>vagas@movemais.com</t>
+  </si>
+  <si>
+    <t>vagas@medibras.com.br</t>
+  </si>
+  <si>
+    <t>recrutamento@newstandard.com.br</t>
+  </si>
+  <si>
+    <t>sinergiadho@outlook.com.br</t>
+  </si>
+  <si>
+    <t>rh@supley.com.br</t>
+  </si>
+  <si>
+    <t>ciee.araraquara@ciee.ong.br</t>
+  </si>
+  <si>
+    <t>145.selecao@gmail.com</t>
+  </si>
+  <si>
+    <t>rh@covizzigestao.com.br</t>
+  </si>
+  <si>
+    <t>recrutamentosp@koandina.com</t>
+  </si>
+  <si>
+    <t>rh@hinove.com</t>
   </si>
 </sst>
 </file>
@@ -68,16 +206,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -356,15 +497,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -382,11 +523,294 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A14" r:id="rId13"/>
+    <hyperlink ref="A15" r:id="rId14"/>
+    <hyperlink ref="A16" r:id="rId15"/>
+    <hyperlink ref="A17" r:id="rId16"/>
+    <hyperlink ref="A18" r:id="rId17"/>
+    <hyperlink ref="A19" r:id="rId18"/>
+    <hyperlink ref="A20" r:id="rId19"/>
+    <hyperlink ref="A21" r:id="rId20"/>
+    <hyperlink ref="A22" r:id="rId21"/>
+    <hyperlink ref="A23" r:id="rId22"/>
+    <hyperlink ref="A24" r:id="rId23"/>
+    <hyperlink ref="A25" r:id="rId24"/>
+    <hyperlink ref="A26" r:id="rId25"/>
+    <hyperlink ref="A27" r:id="rId26"/>
+    <hyperlink ref="A28" r:id="rId27"/>
+    <hyperlink ref="A29" r:id="rId28" display="mailto:recrutamento@jobterceirizacao.com.br"/>
+    <hyperlink ref="A30" r:id="rId29"/>
+    <hyperlink ref="A31" r:id="rId30"/>
+    <hyperlink ref="A32" r:id="rId31"/>
+    <hyperlink ref="A33" r:id="rId32"/>
+    <hyperlink ref="A34" r:id="rId33"/>
+    <hyperlink ref="A35" r:id="rId34"/>
+    <hyperlink ref="A36" r:id="rId35" display="mailto:pessoas@stepwise.com.br"/>
+    <hyperlink ref="A37" r:id="rId36"/>
+    <hyperlink ref="A38" r:id="rId37"/>
+    <hyperlink ref="A39" r:id="rId38"/>
+    <hyperlink ref="A40" r:id="rId39"/>
+    <hyperlink ref="A41" r:id="rId40"/>
+    <hyperlink ref="A42" r:id="rId41"/>
+    <hyperlink ref="A43" r:id="rId42"/>
+    <hyperlink ref="A44" r:id="rId43"/>
+    <hyperlink ref="A45" r:id="rId44" display="mailto:ciee.araraquara@ciee.ong.br"/>
+    <hyperlink ref="A46" r:id="rId45"/>
+    <hyperlink ref="A47" r:id="rId46"/>
+    <hyperlink ref="A48" r:id="rId47"/>
+    <hyperlink ref="A49" r:id="rId48"/>
+    <hyperlink ref="A50" r:id="rId49"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId50"/>
 </worksheet>
 </file>
</xml_diff>